<commit_message>
Add backtesting module and results for portfolio analysis
Added Backtesting.py for comparing stochastic and robust optimization portfolios against S&P 500. Included new result files, configuration, metrics, and supporting data for backtesting and analysis workflows.
</commit_message>
<xml_diff>
--- a/Corridas/20251025_150353_analisis_sp500/resultados.xlsx
+++ b/Corridas/20251025_150353_analisis_sp500/resultados.xlsx
@@ -427,7 +427,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,81 +450,91 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Rendimiento_Esperado</t>
+          <t>Rendimiento_Esperado_Log</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.0396345352594405</v>
+        <v>0.01573400932611407</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Volatilidad</t>
+          <t>Rendimiento_Esperado_Porcentual</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.0648218327808676</v>
+        <v>0.01585844059520181</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Sharpe_Ratio</t>
+          <t>Volatilidad</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.5600150500036709</v>
+        <v>0.03917389605175114</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Riesgo_Varianza</t>
+          <t>Sharpe_Ratio</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.004201870005070761</v>
+        <v>0.3165545744134992</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CVaR_Portafolio</t>
+          <t>Riesgo_Varianza</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>-0.06759962693221996</v>
+        <v>0.001534594131873403</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Funcion_Objetivo</t>
+          <t>CVaR_Portafolio</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.4314190035058122</v>
+        <v>-0.03382977644364061</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>N_Acciones</t>
+          <t>Funcion_Objetivo</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>10</v>
+        <v>0.05679026405857873</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>N_Acciones</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>Peso_Total_Acciones</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>1</v>
+      <c r="B10" t="n">
+        <v>0.9999999999999998</v>
       </c>
     </row>
   </sheetData>
@@ -538,7 +548,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -559,25 +569,30 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Rendimiento_Esperado</t>
+          <t>Rendimiento_Log</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
+          <t>Rendimiento_Porcentual</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>Desvio_Estandar</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>VaR_95</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>CVaR_95</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>Prob_Perdida</t>
         </is>
@@ -586,251 +601,281 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>AVGO</t>
+          <t>RSG</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>0.3</v>
       </c>
       <c r="C2" t="n">
-        <v>0.03970227606524487</v>
+        <v>0.01593411162495392</v>
       </c>
       <c r="D2" t="n">
-        <v>0.09136170361915237</v>
+        <v>0.01606173654377585</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.105931453055878</v>
+        <v>0.04897055828025669</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.1515593398400087</v>
+        <v>-0.06009945731390331</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3525292028344601</v>
+        <v>-0.08589280382996545</v>
+      </c>
+      <c r="H2" t="n">
+        <v>0.3652062211561631</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>LLY</t>
+          <t>MCD</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.3</v>
+        <v>0.2485366752572068</v>
       </c>
       <c r="C3" t="n">
-        <v>0.03532633271988238</v>
+        <v>0.01105134070186723</v>
       </c>
       <c r="D3" t="n">
-        <v>0.07642567826879772</v>
+        <v>0.01111263234437421</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.08116955916157426</v>
+        <v>0.0511631372545762</v>
       </c>
       <c r="F3" t="n">
-        <v>-0.116061859619291</v>
+        <v>-0.05953797337572052</v>
       </c>
       <c r="G3" t="n">
-        <v>0.3653204385164766</v>
+        <v>-0.08479405149596911</v>
+      </c>
+      <c r="H3" t="n">
+        <v>0.378843061609838</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>AXON</t>
+          <t>MMC</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.05</v>
+        <v>0.1014633247427929</v>
       </c>
       <c r="C4" t="n">
-        <v>0.03047847267056679</v>
+        <v>0.01115662774737973</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1073636751944956</v>
+        <v>0.01121909501058549</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.1970602273837241</v>
+        <v>0.05354270517980156</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.2709528289917361</v>
+        <v>-0.06283680939995701</v>
       </c>
       <c r="G4" t="n">
-        <v>0.434626366409078</v>
+        <v>-0.09090181999418419</v>
+      </c>
+      <c r="H4" t="n">
+        <v>0.3492962149470633</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BLDR</t>
+          <t>AJG</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>0.05</v>
       </c>
       <c r="C5" t="n">
-        <v>0.04945074001048379</v>
+        <v>0.01577129163518248</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1328454784763561</v>
+        <v>0.01589631484956922</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.2187073316716535</v>
+        <v>0.05840188965830416</v>
       </c>
       <c r="F5" t="n">
-        <v>-0.3036743819905508</v>
+        <v>-0.06845050899881583</v>
       </c>
       <c r="G5" t="n">
-        <v>0.4196344881723245</v>
+        <v>-0.09831927763281612</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0.3640652192290516</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>DECK</t>
+          <t>COST</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>0.05</v>
       </c>
       <c r="C6" t="n">
-        <v>0.033750691893642</v>
+        <v>0.02031154968988277</v>
       </c>
       <c r="D6" t="n">
-        <v>0.07505165247517273</v>
+        <v>0.02051923295500946</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.1538339743222732</v>
+        <v>0.06575729349546175</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.2138670400299816</v>
+        <v>-0.06992220936854815</v>
       </c>
       <c r="G6" t="n">
-        <v>0.4107879479554503</v>
+        <v>-0.09975833595823232</v>
+      </c>
+      <c r="H6" t="n">
+        <v>0.3523794465681823</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>FICO</t>
+          <t>CTAS</t>
         </is>
       </c>
       <c r="B7" t="n">
         <v>0.05</v>
       </c>
       <c r="C7" t="n">
-        <v>0.04104191691810911</v>
+        <v>0.02303776214964436</v>
       </c>
       <c r="D7" t="n">
-        <v>0.09734722828214223</v>
+        <v>0.02330518102099788</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.1112698480431549</v>
+        <v>0.06352659485413112</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.1579400662961019</v>
+        <v>-0.07606359437629205</v>
       </c>
       <c r="G7" t="n">
-        <v>0.3719254716699139</v>
+        <v>-0.1095501084668015</v>
+      </c>
+      <c r="H7" t="n">
+        <v>0.3424831250497379</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>JBL</t>
+          <t>LLY</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>0.05</v>
       </c>
       <c r="C8" t="n">
-        <v>0.03405407917101086</v>
+        <v>0.03532633271988238</v>
       </c>
       <c r="D8" t="n">
-        <v>0.08956148804463672</v>
+        <v>0.03595772054510604</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.1408906384360055</v>
+        <v>0.07642567826879772</v>
       </c>
       <c r="F8" t="n">
-        <v>-0.1961225802333248</v>
+        <v>-0.08116955916157426</v>
       </c>
       <c r="G8" t="n">
-        <v>0.4292426891362875</v>
+        <v>-0.116061859619291</v>
+      </c>
+      <c r="H8" t="n">
+        <v>0.3653204385164766</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>NVDA</t>
+          <t>PGR</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>0.05</v>
       </c>
       <c r="C9" t="n">
-        <v>0.04632187030857726</v>
+        <v>0.01856688928963813</v>
       </c>
       <c r="D9" t="n">
-        <v>0.1453918229191584</v>
+        <v>0.01874032570732598</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.1702214476978665</v>
+        <v>0.05532539794482709</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.2421981990339286</v>
+        <v>-0.07526015336134566</v>
       </c>
       <c r="G9" t="n">
-        <v>0.3854030242067506</v>
+        <v>-0.1078942195780875</v>
+      </c>
+      <c r="H9" t="n">
+        <v>0.3652459514316563</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>PHM</t>
+          <t>TJX</t>
         </is>
       </c>
       <c r="B10" t="n">
         <v>0.05</v>
       </c>
       <c r="C10" t="n">
-        <v>0.03829590290755464</v>
+        <v>0.01631437673927512</v>
       </c>
       <c r="D10" t="n">
-        <v>0.104804997328068</v>
+        <v>0.01644818284754712</v>
       </c>
       <c r="E10" t="n">
-        <v>-0.1508877826400044</v>
+        <v>0.05931325343532361</v>
       </c>
       <c r="F10" t="n">
-        <v>-0.2110245591182368</v>
+        <v>-0.07222838272756965</v>
       </c>
       <c r="G10" t="n">
-        <v>0.4157691984127205</v>
+        <v>-0.1033520595563616</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.3634465622327827</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>SMCI</t>
+          <t>WRB</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>0.05</v>
       </c>
       <c r="C11" t="n">
-        <v>0.06912537859810222</v>
+        <v>0.01217427416218126</v>
       </c>
       <c r="D11" t="n">
-        <v>0.1928667240180445</v>
+        <v>0.01224868228624798</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.201413019211584</v>
+        <v>0.05513970027329756</v>
       </c>
       <c r="F11" t="n">
-        <v>-0.2770699039679125</v>
+        <v>-0.06722891743011217</v>
       </c>
       <c r="G11" t="n">
-        <v>0.4329677212740458</v>
+        <v>-0.09645117124281785</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.3777689387914418</v>
       </c>
     </row>
   </sheetData>

</xml_diff>